<commit_message>
Plot and fit modified
</commit_message>
<xml_diff>
--- a/data_droplets.xlsx
+++ b/data_droplets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Notebooks\log_norm_fit_on_github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oloehman\Documents\Jupyter-Notebooks\log_norm_fit_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B7E2B6-996A-4F2F-BC92-409E8A94268C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518A4F7E-9BC1-4404-A4DA-4CF0AC7666A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2550" yWindow="300" windowWidth="21600" windowHeight="14070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Sample name</t>
   </si>
   <si>
-    <t>(Q/k)^1/2</t>
-  </si>
-  <si>
     <t>Measurement date</t>
   </si>
   <si>
@@ -72,6 +69,45 @@
   </si>
   <si>
     <t>Concentration (g/ml)</t>
+  </si>
+  <si>
+    <t>k_2000_q_50</t>
+  </si>
+  <si>
+    <t>k_2000_q_100</t>
+  </si>
+  <si>
+    <t>k_2000_q_200</t>
+  </si>
+  <si>
+    <t>k_2000_q_300</t>
+  </si>
+  <si>
+    <t>k_2000_q_500</t>
+  </si>
+  <si>
+    <t>k_1500_q_200</t>
+  </si>
+  <si>
+    <t>k_1500_q_250</t>
+  </si>
+  <si>
+    <t>k_2500_q_150</t>
+  </si>
+  <si>
+    <t>k_2500_q_200</t>
+  </si>
+  <si>
+    <t>k_2500_q_250</t>
+  </si>
+  <si>
+    <t>k_2500_q_300</t>
+  </si>
+  <si>
+    <t>k_2500_q_350</t>
+  </si>
+  <si>
+    <t>(Q/k)</t>
   </si>
 </sst>
 </file>
@@ -148,8 +184,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CBC0EE68-1D7B-4B83-B2A4-8018B16609C8}" name="Tabelle1" displayName="Tabelle1" ref="A1:L3" totalsRowShown="0">
-  <autoFilter ref="A1:L3" xr:uid="{49062C35-B54A-4C17-AB49-AA5A8262EA11}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CBC0EE68-1D7B-4B83-B2A4-8018B16609C8}" name="Tabelle1" displayName="Tabelle1" ref="A1:L14" totalsRowShown="0">
+  <autoFilter ref="A1:L14" xr:uid="{49062C35-B54A-4C17-AB49-AA5A8262EA11}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L14">
+    <sortCondition ref="G1:G14"/>
+  </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{337D852C-D5A8-4BF7-A5B6-91ED956C340D}" name="Sample name"/>
     <tableColumn id="7" xr3:uid="{B7D9AD6B-0E2B-40DD-9CFD-9063325986F3}" name="Measurement date"/>
@@ -159,8 +198,8 @@
     </tableColumn>
     <tableColumn id="2" xr3:uid="{55619954-958C-45A5-95D7-47F60C5A3D6F}" name="Conductivity [S/m]"/>
     <tableColumn id="3" xr3:uid="{1C4D98B3-F14D-4DEF-9A2B-131BE935A54E}" name="Flow [nl/min]"/>
-    <tableColumn id="4" xr3:uid="{FFF52163-286F-47F5-AB15-15920D121761}" name="(Q/k)^1/2" dataDxfId="2">
-      <calculatedColumnFormula>SQRT(Tabelle1[[#This Row],[Flow '[nl/min']]]/Tabelle1[[#This Row],[Conductivity '[S/m']]])</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{FFF52163-286F-47F5-AB15-15920D121761}" name="(Q/k)" dataDxfId="2">
+      <calculatedColumnFormula>Tabelle1[[#This Row],[Flow '[nl/min']]]/Tabelle1[[#This Row],[Conductivity '[S/m']]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{CB02B4BF-4204-4E6C-9E47-72A8500FBD8C}" name="Repetions"/>
     <tableColumn id="5" xr3:uid="{A38B2268-4B71-4BBC-9D11-4353C36325BF}" name="Particle Size  [nm]"/>
@@ -439,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,45 +505,45 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
         <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1">
-        <v>44218</v>
+        <v>44217</v>
       </c>
       <c r="C2">
         <v>1.58E-3</v>
@@ -514,70 +553,535 @@
         <v>1E-3</v>
       </c>
       <c r="E2">
-        <v>0.14580000000000001</v>
+        <v>0.1903</v>
       </c>
       <c r="F2">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="G2">
-        <f>SQRT(Tabelle1[[#This Row],[Flow '[nl/min']]]/Tabelle1[[#This Row],[Conductivity '[S/m']]])</f>
-        <v>45.360921162651444</v>
+        <f>Tabelle1[[#This Row],[Flow '[nl/min']]]/Tabelle1[[#This Row],[Conductivity '[S/m']]]</f>
+        <v>262.74303730951129</v>
       </c>
       <c r="H2">
         <v>2</v>
       </c>
       <c r="I2">
+        <v>12.33</v>
+      </c>
+      <c r="J2">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="K2">
+        <f>Tabelle1[[#This Row],[Particle Size  '[nm']]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>123.29999999999998</v>
+      </c>
+      <c r="L2">
+        <f>Tabelle1[[#This Row],[Deviation Particle]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44217</v>
+      </c>
+      <c r="C3">
+        <v>1.58E-3</v>
+      </c>
+      <c r="D3">
+        <f>Tabelle1[[#This Row],[Concentration (g/ml)]]/(1.58)</f>
+        <v>1E-3</v>
+      </c>
+      <c r="E3">
+        <v>0.1903</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <f>Tabelle1[[#This Row],[Flow '[nl/min']]]/Tabelle1[[#This Row],[Conductivity '[S/m']]]</f>
+        <v>525.48607461902259</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>15.2</v>
+      </c>
+      <c r="J3">
+        <v>1.375</v>
+      </c>
+      <c r="K3">
+        <f>Tabelle1[[#This Row],[Particle Size  '[nm']]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>151.99999999999997</v>
+      </c>
+      <c r="L3">
+        <f>Tabelle1[[#This Row],[Deviation Particle]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>13.749999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44228</v>
+      </c>
+      <c r="C4">
+        <v>1.57E-3</v>
+      </c>
+      <c r="D4">
+        <f>Tabelle1[[#This Row],[Concentration (g/ml)]]/(1.58)</f>
+        <v>9.9367088607594926E-4</v>
+      </c>
+      <c r="E4">
+        <v>0.255</v>
+      </c>
+      <c r="F4">
+        <v>150</v>
+      </c>
+      <c r="G4">
+        <f>Tabelle1[[#This Row],[Flow '[nl/min']]]/Tabelle1[[#This Row],[Conductivity '[S/m']]]</f>
+        <v>588.23529411764707</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>7.18</v>
+      </c>
+      <c r="J4">
+        <v>1.17</v>
+      </c>
+      <c r="K4">
+        <f>Tabelle1[[#This Row],[Particle Size  '[nm']]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>71.952119098793801</v>
+      </c>
+      <c r="L4">
+        <f>Tabelle1[[#This Row],[Deviation Particle]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>11.724788209692026</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44228</v>
+      </c>
+      <c r="C5">
+        <v>1.57E-3</v>
+      </c>
+      <c r="D5">
+        <f>Tabelle1[[#This Row],[Concentration (g/ml)]]/(1.58)</f>
+        <v>9.9367088607594926E-4</v>
+      </c>
+      <c r="E5">
+        <v>0.255</v>
+      </c>
+      <c r="F5">
+        <v>200</v>
+      </c>
+      <c r="G5">
+        <f>Tabelle1[[#This Row],[Flow '[nl/min']]]/Tabelle1[[#This Row],[Conductivity '[S/m']]]</f>
+        <v>784.31372549019602</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>10.653</v>
+      </c>
+      <c r="J5">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="K5">
+        <f>Tabelle1[[#This Row],[Particle Size  '[nm']]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>106.75569982722151</v>
+      </c>
+      <c r="L5">
+        <f>Tabelle1[[#This Row],[Deviation Particle]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>11.223728884491512</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44228</v>
+      </c>
+      <c r="C6">
+        <v>1.57E-3</v>
+      </c>
+      <c r="D6">
+        <f>Tabelle1[[#This Row],[Concentration (g/ml)]]/(1.58)</f>
+        <v>9.9367088607594926E-4</v>
+      </c>
+      <c r="E6">
+        <v>0.255</v>
+      </c>
+      <c r="F6">
+        <v>250</v>
+      </c>
+      <c r="G6">
+        <f>Tabelle1[[#This Row],[Flow '[nl/min']]]/Tabelle1[[#This Row],[Conductivity '[S/m']]]</f>
+        <v>980.39215686274508</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>9.3569999999999993</v>
+      </c>
+      <c r="J6">
+        <v>1.135</v>
+      </c>
+      <c r="K6">
+        <f>Tabelle1[[#This Row],[Particle Size  '[nm']]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>93.768242118024176</v>
+      </c>
+      <c r="L6">
+        <f>Tabelle1[[#This Row],[Deviation Particle]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>11.374046682051667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44217</v>
+      </c>
+      <c r="C7">
+        <v>1.58E-3</v>
+      </c>
+      <c r="D7">
+        <f>Tabelle1[[#This Row],[Concentration (g/ml)]]/(1.58)</f>
+        <v>1E-3</v>
+      </c>
+      <c r="E7">
+        <v>0.1903</v>
+      </c>
+      <c r="F7">
+        <v>200</v>
+      </c>
+      <c r="G7">
+        <f>Tabelle1[[#This Row],[Flow '[nl/min']]]/Tabelle1[[#This Row],[Conductivity '[S/m']]]</f>
+        <v>1050.9721492380452</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>16.55</v>
+      </c>
+      <c r="J7">
+        <v>1.2150000000000001</v>
+      </c>
+      <c r="K7">
+        <f>Tabelle1[[#This Row],[Particle Size  '[nm']]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>165.49999999999997</v>
+      </c>
+      <c r="L7">
+        <f>Tabelle1[[#This Row],[Deviation Particle]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>12.149999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44228</v>
+      </c>
+      <c r="C8">
+        <v>1.57E-3</v>
+      </c>
+      <c r="D8">
+        <f>Tabelle1[[#This Row],[Concentration (g/ml)]]/(1.58)</f>
+        <v>9.9367088607594926E-4</v>
+      </c>
+      <c r="E8">
+        <v>0.255</v>
+      </c>
+      <c r="F8">
+        <v>300</v>
+      </c>
+      <c r="G8">
+        <f>Tabelle1[[#This Row],[Flow '[nl/min']]]/Tabelle1[[#This Row],[Conductivity '[S/m']]]</f>
+        <v>1176.4705882352941</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>11.372999999999999</v>
+      </c>
+      <c r="J8">
+        <v>1.093</v>
+      </c>
+      <c r="K8">
+        <f>Tabelle1[[#This Row],[Particle Size  '[nm']]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>113.97095411010889</v>
+      </c>
+      <c r="L8">
+        <f>Tabelle1[[#This Row],[Deviation Particle]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>10.953156848883234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44218</v>
+      </c>
+      <c r="C9">
+        <v>1.58E-3</v>
+      </c>
+      <c r="D9">
+        <f>Tabelle1[[#This Row],[Concentration (g/ml)]]/(1.58)</f>
+        <v>1E-3</v>
+      </c>
+      <c r="E9">
+        <v>0.14580000000000001</v>
+      </c>
+      <c r="F9">
+        <v>200</v>
+      </c>
+      <c r="G9">
+        <f>Tabelle1[[#This Row],[Flow '[nl/min']]]/Tabelle1[[#This Row],[Conductivity '[S/m']]]</f>
+        <v>1371.7421124828531</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>17.754999999999999</v>
+      </c>
+      <c r="J9">
+        <v>1.2350000000000001</v>
+      </c>
+      <c r="K9">
+        <f>Tabelle1[[#This Row],[Particle Size  '[nm']]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>177.54999999999995</v>
+      </c>
+      <c r="L9">
+        <f>Tabelle1[[#This Row],[Deviation Particle]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>12.349999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44228</v>
+      </c>
+      <c r="C10">
+        <v>1.57E-3</v>
+      </c>
+      <c r="D10">
+        <f>Tabelle1[[#This Row],[Concentration (g/ml)]]/(1.58)</f>
+        <v>9.9367088607594926E-4</v>
+      </c>
+      <c r="E10">
+        <v>0.255</v>
+      </c>
+      <c r="F10">
+        <v>350</v>
+      </c>
+      <c r="G10">
+        <f>Tabelle1[[#This Row],[Flow '[nl/min']]]/Tabelle1[[#This Row],[Conductivity '[S/m']]]</f>
+        <v>1372.5490196078431</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>11.186</v>
+      </c>
+      <c r="J10">
+        <v>1.0980000000000001</v>
+      </c>
+      <c r="K10">
+        <f>Tabelle1[[#This Row],[Particle Size  '[nm']]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>112.09699223385897</v>
+      </c>
+      <c r="L10">
+        <f>Tabelle1[[#This Row],[Deviation Particle]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>11.003262781403286</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44217</v>
+      </c>
+      <c r="C11">
+        <v>1.58E-3</v>
+      </c>
+      <c r="D11">
+        <f>Tabelle1[[#This Row],[Concentration (g/ml)]]/(1.58)</f>
+        <v>1E-3</v>
+      </c>
+      <c r="E11">
+        <v>0.1903</v>
+      </c>
+      <c r="F11">
+        <v>300</v>
+      </c>
+      <c r="G11">
+        <f>Tabelle1[[#This Row],[Flow '[nl/min']]]/Tabelle1[[#This Row],[Conductivity '[S/m']]]</f>
+        <v>1576.4582238570679</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>15.305</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="K11">
+        <f>Tabelle1[[#This Row],[Particle Size  '[nm']]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>153.04999999999995</v>
+      </c>
+      <c r="L11">
+        <f>Tabelle1[[#This Row],[Deviation Particle]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>11.999999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44218</v>
+      </c>
+      <c r="C12">
+        <v>1.58E-3</v>
+      </c>
+      <c r="D12">
+        <f>Tabelle1[[#This Row],[Concentration (g/ml)]]/(1.58)</f>
+        <v>1E-3</v>
+      </c>
+      <c r="E12">
+        <v>0.14580000000000001</v>
+      </c>
+      <c r="F12">
+        <v>250</v>
+      </c>
+      <c r="G12">
+        <f>Tabelle1[[#This Row],[Flow '[nl/min']]]/Tabelle1[[#This Row],[Conductivity '[S/m']]]</f>
+        <v>1714.6776406035665</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>19.605</v>
+      </c>
+      <c r="J12">
+        <v>1.1950000000000001</v>
+      </c>
+      <c r="K12">
+        <f>Tabelle1[[#This Row],[Particle Size  '[nm']]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>196.04999999999995</v>
+      </c>
+      <c r="L12">
+        <f>Tabelle1[[#This Row],[Deviation Particle]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>11.949999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44218</v>
+      </c>
+      <c r="C13">
+        <v>1.58E-3</v>
+      </c>
+      <c r="D13">
+        <f>Tabelle1[[#This Row],[Concentration (g/ml)]]/(1.58)</f>
+        <v>1E-3</v>
+      </c>
+      <c r="E13">
+        <v>0.14580000000000001</v>
+      </c>
+      <c r="F13">
+        <v>300</v>
+      </c>
+      <c r="G13">
+        <f>Tabelle1[[#This Row],[Flow '[nl/min']]]/Tabelle1[[#This Row],[Conductivity '[S/m']]]</f>
+        <v>2057.6131687242796</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
         <v>21.25</v>
       </c>
-      <c r="J2">
+      <c r="J13">
         <v>1.2</v>
       </c>
-      <c r="K2">
+      <c r="K13">
         <f>Tabelle1[[#This Row],[Particle Size  '[nm']]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
         <v>212.49999999999997</v>
       </c>
-      <c r="L2">
+      <c r="L13">
         <f>Tabelle1[[#This Row],[Deviation Particle]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
         <v>11.999999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>1E-4</v>
-      </c>
-      <c r="D3" s="2">
-        <f>Tabelle1[[#This Row],[Concentration (g/ml)]]/(1.58)</f>
-        <v>6.3291139240506333E-5</v>
-      </c>
-      <c r="E3">
-        <v>1E-4</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <f>SQRT(Tabelle1[[#This Row],[Flow '[nl/min']]]/Tabelle1[[#This Row],[Conductivity '[S/m']]])</f>
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2">
-        <f>Tabelle1[[#This Row],[Particle Size  '[nm']]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
-        <v>0</v>
-      </c>
-      <c r="L3" s="2">
-        <f>Tabelle1[[#This Row],[Deviation Particle]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
-        <v>0</v>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44217</v>
+      </c>
+      <c r="C14">
+        <v>1.58E-3</v>
+      </c>
+      <c r="D14">
+        <f>Tabelle1[[#This Row],[Concentration (g/ml)]]/(1.58)</f>
+        <v>1E-3</v>
+      </c>
+      <c r="E14">
+        <v>0.1903</v>
+      </c>
+      <c r="F14">
+        <v>500</v>
+      </c>
+      <c r="G14">
+        <f>Tabelle1[[#This Row],[Flow '[nl/min']]]/Tabelle1[[#This Row],[Conductivity '[S/m']]]</f>
+        <v>2627.4303730951128</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <v>15.43</v>
+      </c>
+      <c r="J14">
+        <v>1.26</v>
+      </c>
+      <c r="K14">
+        <f>Tabelle1[[#This Row],[Particle Size  '[nm']]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>154.29999999999995</v>
+      </c>
+      <c r="L14">
+        <f>Tabelle1[[#This Row],[Deviation Particle]]/POWER(Tabelle1[[#This Row],[Concentration (V/V) '[ml/ml']]],1/3)</f>
+        <v>12.599999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>